<commit_message>
update user operation interface
</commit_message>
<xml_diff>
--- a/数据库表设计.xlsx
+++ b/数据库表设计.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
   <si>
     <t>字段</t>
   </si>
@@ -88,6 +88,9 @@
     <t>请假天数</t>
   </si>
   <si>
+    <t>requesterId</t>
+  </si>
+  <si>
     <t>连线表lineData</t>
   </si>
   <si>
@@ -148,9 +151,6 @@
     <t>数据表单id</t>
   </si>
   <si>
-    <t>requesterId</t>
-  </si>
-  <si>
     <t>流程发起人id</t>
   </si>
   <si>
@@ -158,6 +158,33 @@
   </si>
   <si>
     <t>流程最终结果</t>
+  </si>
+  <si>
+    <t>用户表userData（用户包括申请人，1级处理人，2级处理人等）</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>用户名</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>用户id</t>
+  </si>
+  <si>
+    <t>userPassword</t>
+  </si>
+  <si>
+    <t>用户密码</t>
+  </si>
+  <si>
+    <t>userLevel</t>
+  </si>
+  <si>
+    <t>用户权限（权限从0开始逐渐增加）</t>
   </si>
 </sst>
 </file>
@@ -1120,10 +1147,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="4"/>
@@ -1247,6 +1274,11 @@
         <v>23</v>
       </c>
     </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
@@ -1263,7 +1295,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1279,57 +1311,57 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1343,7 +1375,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1370,13 +1402,13 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1392,13 +1424,13 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1420,7 +1452,7 @@
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1434,7 +1466,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1450,13 +1482,13 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1472,7 +1504,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B39" t="s">
         <v>5</v>
@@ -1490,6 +1522,64 @@
       </c>
       <c r="C40" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>